<commit_message>
feat: added html template styling for questions
</commit_message>
<xml_diff>
--- a/Quantium.Recruitment.Portal/wwwroot/QuestionsTemplate.xlsx
+++ b/Quantium.Recruitment.Portal/wwwroot/QuestionsTemplate.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QRecruitment\newcode\Quantium.Recruitment.Portal\wwwroot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\QuantiumRecruitment\Quantium.Recruitment.Portal\wwwroot\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11385"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11388"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -116,14 +116,6 @@
     <t>Convert.ToString() only handle null values</t>
   </si>
   <si>
-    <t>Which of the following statements are TRUE about the .NET CLR?
-1.It provides a language-neutral development &amp; execution environment.
-2.It ensures that an application would not be able to access memory that it is not authorized to access.
-3.It provides services to run "managed" applications.
-4.The resources are garbage collected.
-It provides services to run "unmanaged" applications.</t>
-  </si>
-  <si>
     <t>Consider the following schema. &lt;i&gt;STUDENTS(student_code, first_name, last_name, email, phone_no, date_of_birth, honours_subject, percentage_of_marks)&lt;/i&gt;</t>
   </si>
   <si>
@@ -242,14 +234,6 @@
   </si>
   <si>
     <t>OOPS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Which of the statements are true ?
-I. Function overloading is done at compile time.
-II. Protected members are accessible to the member of derived class.
-III. A derived class inherits constructors and destructors.
-IV. A friend function can be called like a normal function.
-V. Nested class is a derived class. </t>
   </si>
   <si>
     <t xml:space="preserve"> I, II, III</t>
@@ -352,88 +336,104 @@
     <t>The structure variable b will be created on the stack.</t>
   </si>
   <si>
-    <t xml:space="preserve">Which of the following is NOT an Arithmetic operator in C#.NET?
-A) **
-B) /
-C) +
-D) %
+    <t>A</t>
+  </si>
+  <si>
+    <t>B</t>
+  </si>
+  <si>
+    <t>D</t>
+  </si>
+  <si>
+    <t>E</t>
+  </si>
+  <si>
+    <t>A,E</t>
+  </si>
+  <si>
+    <t>Option-1;Option-5;Option-6</t>
+  </si>
+  <si>
+    <t>All the above</t>
+  </si>
+  <si>
+    <t>4 and 5</t>
+  </si>
+  <si>
+    <t>3 and 4</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1, 2 and 4</t>
+  </si>
+  <si>
+    <t>1 and 2</t>
+  </si>
+  <si>
+    <t>A constructor cannot be declared as private.</t>
+  </si>
+  <si>
+    <t>A constructor cannot be overloaded.</t>
+  </si>
+  <si>
+    <t>A constructor can be a static constructor.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 
+A constructor cannot access static data.</t>
+  </si>
+  <si>
+    <t>Mental break time. This is an easy question. You don’t have to think  too hard to get the right answer for this question. Are you ready? Here we go. What is 1+1?</t>
+  </si>
+  <si>
+    <t>Not this one</t>
+  </si>
+  <si>
+    <t>Still not this one</t>
+  </si>
+  <si>
+    <t>You have gone too far. Go back to option 3</t>
+  </si>
+  <si>
+    <t>Which of the following statements are TRUE about the .NET CLR?&lt;br/&gt;
+1.It provides a language-neutral development &amp; execution environment.&lt;br/&gt;
+2.It ensures that an application would not be able to access memory that it is not authorized to access.&lt;br/&gt;
+3.It provides services to run "managed" applications.&lt;br/&gt;
+4.The resources are garbage collected.&lt;br/&gt;
+5.It provides services to run "unmanaged" applications.</t>
+  </si>
+  <si>
+    <t>Which of the statements are true ?&lt;br/&gt;
+I. Function overloading is done at compile time.&lt;br/&gt;
+II. Protected members are accessible to the member of derived class.&lt;br/&gt;
+III. A derived class inherits constructors and destructors.&lt;br/&gt;
+IV. A friend function can be called like a normal function.&lt;br/&gt;
+&lt;b&gt;V. Nested class is a derived class.&lt;/b&gt; &lt;br/&gt;</t>
+  </si>
+  <si>
+    <t>&lt;b&gt;Which of the following statements are correct about constructors in C#.NET?&lt;/b&gt;&lt;br/&gt;
+1)Constructors cannot be overloaded.&lt;br/&gt;
+2)Constructors always have the name same as the name of the class.&lt;br/&gt;
+3)Constructors are never called explicitly.&lt;br/&gt;
+4)Constructors never return any value.&lt;br/&gt;
+5)Constructors allocate space for the object in memory.&lt;br/&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Which of the following is NOT an Arithmetic operator in C#.NET?&lt;br/&gt;
+A) **&lt;br/&gt;
+B) /&lt;br/&gt;
+C) +&lt;br/&gt;
+D) %&lt;br/&gt;
 E)~
 </t>
   </si>
   <si>
-    <t>A</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
-    <t>D</t>
-  </si>
-  <si>
-    <t>E</t>
-  </si>
-  <si>
-    <t>A,E</t>
-  </si>
-  <si>
-    <t>Option-1;Option-5;Option-6</t>
-  </si>
-  <si>
-    <t>All the above</t>
-  </si>
-  <si>
-    <t>4 and 5</t>
-  </si>
-  <si>
-    <t>3 and 4</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 1, 2 and 4</t>
-  </si>
-  <si>
-    <t>1 and 2</t>
-  </si>
-  <si>
-    <t>Which of the following statements are correct about constructors in C#.NET?
-1)Constructors cannot be overloaded.
-2)Constructors always have the name same as the name of the class.
-3)Constructors are never called explicitly.
-4)Constructors never return any value.
-5)Constructors allocate space for the object in memory.</t>
-  </si>
-  <si>
-    <t>Which of the following statements is correct about constructors in C#.NET?</t>
-  </si>
-  <si>
-    <t>A constructor cannot be declared as private.</t>
-  </si>
-  <si>
-    <t>A constructor cannot be overloaded.</t>
-  </si>
-  <si>
-    <t>A constructor can be a static constructor.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 
-A constructor cannot access static data.</t>
-  </si>
-  <si>
-    <t>Mental break time. This is an easy question. You don’t have to think  too hard to get the right answer for this question. Are you ready? Here we go. What is 1+1?</t>
-  </si>
-  <si>
-    <t>Not this one</t>
-  </si>
-  <si>
-    <t>Still not this one</t>
-  </si>
-  <si>
-    <t>You have gone too far. Go back to option 3</t>
+    <t>&lt;span style="color: #ff0000"&gt;Which of the following statements is correct about constructors in C#.NET?&lt;/span&gt;</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -566,6 +566,23 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -601,6 +618,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -755,24 +789,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A22" sqref="A22:M25"/>
+    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="46.140625" customWidth="1"/>
+    <col min="2" max="2" width="46.109375" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.6640625" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="16.5703125" customWidth="1"/>
-    <col min="8" max="8" width="11.28515625" customWidth="1"/>
-    <col min="13" max="13" width="18.28515625" customWidth="1"/>
+    <col min="6" max="6" width="16.5546875" customWidth="1"/>
+    <col min="8" max="8" width="11.33203125" customWidth="1"/>
+    <col min="13" max="13" width="18.33203125" customWidth="1"/>
     <col min="14" max="14" width="14" customWidth="1"/>
-    <col min="15" max="15" width="20.5703125" customWidth="1"/>
+    <col min="15" max="15" width="20.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -819,7 +853,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -854,7 +888,7 @@
       <c r="N2" s="2"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -891,12 +925,12 @@
       <c r="N3" s="2"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" ht="181.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" ht="147" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>30</v>
+        <v>120</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -905,19 +939,19 @@
         <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>113</v>
+        <v>110</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>112</v>
+        <v>109</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>111</v>
+        <v>108</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1" t="s">
@@ -932,12 +966,12 @@
       <c r="N4" s="2"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>15</v>
@@ -946,16 +980,16 @@
         <v>56</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F5" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="G5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="G5" s="1" t="s">
+      <c r="H5" s="2" t="s">
         <v>34</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>35</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -970,39 +1004,39 @@
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D6" s="1">
         <v>172</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="G6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>39</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>40</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>41</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>16</v>
@@ -1015,15 +1049,15 @@
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
@@ -1032,16 +1066,16 @@
         <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>43</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="G7" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G7" s="1" t="s">
+      <c r="H7" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>46</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -1056,33 +1090,33 @@
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D8" s="1">
         <v>56</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="F8" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="2" t="s">
         <v>49</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>50</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -1097,15 +1131,15 @@
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>4</v>
@@ -1114,16 +1148,16 @@
         <v>172</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="F9" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="G9" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="G9" s="1" t="s">
+      <c r="H9" s="2" t="s">
         <v>54</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>55</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1138,15 +1172,15 @@
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
@@ -1155,10 +1189,10 @@
         <v>23</v>
       </c>
       <c r="E10" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>62</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>63</v>
       </c>
       <c r="G10" s="1">
         <v>4</v>
@@ -1173,7 +1207,7 @@
         <v>10</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>19</v>
@@ -1186,12 +1220,12 @@
       </c>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>6</v>
@@ -1200,21 +1234,21 @@
         <v>56</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F11" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="F11" s="3" t="s">
+      <c r="G11" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>67</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>68</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L11" s="1" t="s">
         <v>19</v>
@@ -1225,12 +1259,12 @@
       <c r="N11" s="2"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:15" ht="150" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:15" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>71</v>
+        <v>121</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>7</v>
@@ -1239,21 +1273,21 @@
         <v>172</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>73</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>75</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>17</v>
@@ -1264,12 +1298,12 @@
       <c r="N12" s="2"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>7</v>
@@ -1278,21 +1312,21 @@
         <v>23</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="H13" s="2" t="s">
         <v>78</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>80</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="L13" s="1" t="s">
         <v>22</v>
@@ -1303,12 +1337,12 @@
       <c r="N13" s="2"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>6</v>
@@ -1323,15 +1357,15 @@
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>17</v>
@@ -1344,12 +1378,12 @@
       </c>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>7</v>
@@ -1358,21 +1392,21 @@
         <v>172</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="H15" s="2" t="s">
         <v>87</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>88</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>89</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L15" s="1" t="s">
         <v>19</v>
@@ -1385,12 +1419,12 @@
       </c>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>4</v>
@@ -1399,25 +1433,25 @@
         <v>23</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>97</v>
-      </c>
       <c r="K16" s="1" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="L16" s="1" t="s">
         <v>22</v>
@@ -1430,12 +1464,12 @@
       </c>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>7</v>
@@ -1444,16 +1478,16 @@
         <v>56</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="H17" s="2" t="s">
         <v>100</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>102</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
@@ -1469,36 +1503,36 @@
       <c r="N17" s="2"/>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="1:15" ht="120" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>103</v>
+        <v>123</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="D18" s="1">
         <v>172</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H18" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>105</v>
-      </c>
-      <c r="G18" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>106</v>
-      </c>
-      <c r="I18" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>108</v>
       </c>
       <c r="K18" s="1" t="s">
         <v>21</v>
@@ -1512,12 +1546,12 @@
       <c r="N18" s="2"/>
       <c r="O18" s="1"/>
     </row>
-    <row r="19" spans="1:15" ht="135" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:15" ht="129.6" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>115</v>
+        <v>122</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>4</v>
@@ -1535,7 +1569,7 @@
         <v>4</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
@@ -1551,12 +1585,12 @@
       <c r="N19" s="2"/>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>116</v>
+        <v>124</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>6</v>
@@ -1565,16 +1599,16 @@
         <v>56</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>117</v>
+        <v>112</v>
       </c>
       <c r="F20" s="1" t="s">
-        <v>118</v>
+        <v>113</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>119</v>
+        <v>114</v>
       </c>
       <c r="H20" s="3" t="s">
-        <v>120</v>
+        <v>115</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
@@ -1590,12 +1624,12 @@
       <c r="N20" s="2"/>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>6</v>
@@ -1604,16 +1638,16 @@
         <v>172</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>122</v>
+        <v>117</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="G21" s="1">
         <v>2</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>124</v>
+        <v>119</v>
       </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>

</xml_diff>

<commit_message>
fix: changed urls for questions and added chips above questions in preview questions modal
</commit_message>
<xml_diff>
--- a/Quantium.Recruitment.Portal/wwwroot/QuestionsTemplate.xlsx
+++ b/Quantium.Recruitment.Portal/wwwroot/QuestionsTemplate.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Projects\QuantiumRecruitment\Quantium.Recruitment.Portal\wwwroot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QRecruitment\newcode\Quantium.Recruitment.Portal\wwwroot\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11388"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="127">
   <si>
     <t>Id</t>
   </si>
@@ -80,13 +80,7 @@
     <t>Medium</t>
   </si>
   <si>
-    <t>https://s.blogcdn.com/slideshows/images/slides/387/436/1/S3874361/slug/l/game-of-thrones-meme-5-1-2.jpg</t>
-  </si>
-  <si>
     <t>Easy</t>
-  </si>
-  <si>
-    <t>http://9gagofthrones.com/wp-content/uploads/2016/02/jon-snow-subscribe.jpg</t>
   </si>
   <si>
     <t>C#</t>
@@ -435,15 +429,35 @@
         }
 &lt;/pre&gt;</t>
   </si>
+  <si>
+    <t>https://qzxnta.bl3302.livefilestore.com/y3mHsbgprowWwjSXHV1sliJb2WOiL62io-2a3yTs8f74kUgOuUS6V0laeuoIeIvU4SHcUTxPke1u8fSpCwIeMyX026vzHuh6ImXN-99OrTyUZHtW7_t2kHaSvbf7LjWOvVZtK4YjLu1t7UHjoq3wDzFpkPqWmTxIAcnOQUW5zpEr1E?width=665&amp;height=284&amp;cropmode=none</t>
+  </si>
+  <si>
+    <t>https://stxnta.bl3302.livefilestore.com/y3mUg-StpbqNwPznGWzDK8_IXUwJysAMpvKiu1ZSxl8qHy1ZJO_UwAiykFL9wrM80_YBTbpyhJAWG4I4z9eBA7r7rOepD0cqYnYoo1F0jdmNLNzWArI1pkGll4KzXSEtyhViULG4RSLX_xcrGY4iXpxP7MddtWbYCWMzZboTGi2gto?width=667&amp;height=271&amp;cropmode=none</t>
+  </si>
+  <si>
+    <t>https://rdxnta.bl3302.livefilestore.com/y3mvAUDN9Ro6O3Sgz8sugwbfl3pcFvYMnfGt95hIOkCiTYn7adhe5FPojRswD4yeo-t8TCAl65Lbd8eV5f5XEFH_g_hVAJ5RIf_k_wDbRitzJlbIs18V_dPlxkt3CtJPxdUwEhHIpdahDhUotLaCHsr6q0skvtPmQsLjeQ-5myq24g?width=650&amp;height=235&amp;cropmode=none</t>
+  </si>
+  <si>
+    <t>https://qjxnta.bl3302.livefilestore.com/y3mbPGVnlzCISN5I64XFRCEp_zwPHXkgdd_EIGt0xqSKXbq7rhQrrRGSUcyamcjenBxni79zrf9HCS6y4wYwBSSljHN8-DgTHbh2gh2f8dMdvrdZpy2iOpMqOpR8OkeZwWRZrBjamYNEDz_4UGEnGEjmt9EPrmR1PbbkoXmnNKv3vI?width=172&amp;height=144&amp;cropmode=none</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -466,10 +480,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyProtection="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
@@ -479,8 +494,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="fill"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -572,23 +591,6 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri" panose="020F0502020204030204"/>
@@ -624,23 +626,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -795,24 +780,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="N12" sqref="N12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="46.109375" customWidth="1"/>
+    <col min="2" max="2" width="46.140625" customWidth="1"/>
     <col min="3" max="3" width="27" customWidth="1"/>
-    <col min="4" max="4" width="22.6640625" customWidth="1"/>
+    <col min="4" max="4" width="22.7109375" customWidth="1"/>
     <col min="5" max="5" width="11" customWidth="1"/>
-    <col min="6" max="6" width="16.5546875" customWidth="1"/>
-    <col min="8" max="8" width="11.33203125" customWidth="1"/>
-    <col min="13" max="13" width="18.33203125" customWidth="1"/>
+    <col min="6" max="6" width="16.5703125" customWidth="1"/>
+    <col min="8" max="8" width="11.28515625" customWidth="1"/>
+    <col min="13" max="13" width="18.28515625" customWidth="1"/>
     <col min="14" max="14" width="14" customWidth="1"/>
-    <col min="15" max="15" width="20.5546875" customWidth="1"/>
+    <col min="15" max="15" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -859,12 +844,12 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
@@ -873,20 +858,20 @@
         <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M2" s="1" t="b">
         <v>1</v>
@@ -894,12 +879,12 @@
       <c r="N2" s="2"/>
       <c r="O2" s="1"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
@@ -908,22 +893,22 @@
         <v>172</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>27</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>29</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M3" s="1" t="b">
         <v>1</v>
@@ -931,12 +916,12 @@
       <c r="N3" s="2"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" ht="147" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:15" ht="147" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -945,26 +930,26 @@
         <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L4" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M4" s="1" t="b">
         <v>0</v>
@@ -972,12 +957,12 @@
       <c r="N4" s="2"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>15</v>
@@ -986,16 +971,16 @@
         <v>56</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" s="2" t="s">
         <v>32</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>34</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
@@ -1003,67 +988,67 @@
         <v>16</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M5" s="1" t="b">
         <v>1</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D6" s="1">
         <v>172</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>38</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>40</v>
       </c>
       <c r="K6" s="1" t="s">
         <v>16</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M6" s="1" t="b">
         <v>1</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
@@ -1072,16 +1057,16 @@
         <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="H7" s="2" t="s">
         <v>43</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>45</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
@@ -1096,33 +1081,33 @@
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D8" s="1">
         <v>56</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>46</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="H8" s="2" t="s">
         <v>47</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>48</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>49</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
@@ -1137,15 +1122,15 @@
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>4</v>
@@ -1154,16 +1139,16 @@
         <v>172</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="H9" s="2" t="s">
         <v>52</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>54</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
@@ -1171,22 +1156,22 @@
         <v>16</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M9" s="1" t="b">
         <v>1</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="100.8" x14ac:dyDescent="0.3">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
@@ -1195,10 +1180,10 @@
         <v>23</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="G10" s="1">
         <v>4</v>
@@ -1213,25 +1198,25 @@
         <v>10</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M10" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="N10" s="2" t="s">
-        <v>18</v>
+      <c r="N10" s="5" t="s">
+        <v>126</v>
       </c>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>6</v>
@@ -1240,24 +1225,24 @@
         <v>56</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>64</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>65</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>67</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>66</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M11" s="1" t="b">
         <v>1</v>
@@ -1265,12 +1250,12 @@
       <c r="N11" s="2"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:15" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:15" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>7</v>
@@ -1279,21 +1264,21 @@
         <v>172</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>72</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="L12" s="1" t="s">
         <v>17</v>
@@ -1304,12 +1289,12 @@
       <c r="N12" s="2"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>7</v>
@@ -1318,24 +1303,24 @@
         <v>23</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="H13" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>76</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>77</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M13" s="1" t="b">
         <v>1</v>
@@ -1343,12 +1328,12 @@
       <c r="N13" s="2"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>6</v>
@@ -1363,15 +1348,15 @@
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="L14" s="1" t="s">
         <v>17</v>
@@ -1379,17 +1364,17 @@
       <c r="M14" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="N14" s="2" t="s">
-        <v>20</v>
+      <c r="N14" s="5" t="s">
+        <v>125</v>
       </c>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>7</v>
@@ -1398,39 +1383,39 @@
         <v>172</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="H15" s="2" t="s">
         <v>84</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>85</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>86</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M15" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="N15" s="2" t="s">
-        <v>20</v>
+      <c r="N15" s="5" t="s">
+        <v>124</v>
       </c>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>4</v>
@@ -1439,43 +1424,43 @@
         <v>23</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>93</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>94</v>
-      </c>
       <c r="K16" s="1" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="M16" s="1" t="b">
         <v>1</v>
       </c>
-      <c r="N16" s="2" t="s">
-        <v>20</v>
+      <c r="N16" s="5" t="s">
+        <v>123</v>
       </c>
       <c r="O16" s="1"/>
     </row>
-    <row r="17" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:15" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="1">
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>7</v>
@@ -1484,21 +1469,21 @@
         <v>56</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="H17" s="2" t="s">
         <v>97</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>99</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L17" s="1" t="s">
         <v>17</v>
@@ -1509,42 +1494,42 @@
       <c r="N17" s="2"/>
       <c r="O17" s="1"/>
     </row>
-    <row r="18" spans="1:15" ht="115.2" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:15" ht="120" x14ac:dyDescent="0.25">
       <c r="A18" s="1">
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="D18" s="1">
         <v>172</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="H18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>103</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>104</v>
-      </c>
       <c r="K18" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M18" s="1" t="b">
         <v>1</v>
@@ -1552,12 +1537,12 @@
       <c r="N18" s="2"/>
       <c r="O18" s="1"/>
     </row>
-    <row r="19" spans="1:15" ht="129.6" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:15" ht="135" x14ac:dyDescent="0.25">
       <c r="A19" s="1">
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>4</v>
@@ -1575,15 +1560,15 @@
         <v>4</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M19" s="1" t="b">
         <v>0</v>
@@ -1591,12 +1576,12 @@
       <c r="N19" s="2"/>
       <c r="O19" s="1"/>
     </row>
-    <row r="20" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:15" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="1">
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>6</v>
@@ -1605,21 +1590,21 @@
         <v>56</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="H20" s="3" t="s">
         <v>112</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>113</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>114</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L20" s="1" t="s">
         <v>17</v>
@@ -1630,12 +1615,12 @@
       <c r="N20" s="2"/>
       <c r="O20" s="1"/>
     </row>
-    <row r="21" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:15" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="1">
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>6</v>
@@ -1644,24 +1629,24 @@
         <v>172</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="G21" s="1">
         <v>2</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="M21" s="1" t="b">
         <v>0</v>
@@ -1670,7 +1655,13 @@
       <c r="O21" s="1"/>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="N16" r:id="rId1"/>
+    <hyperlink ref="N15" r:id="rId2"/>
+    <hyperlink ref="N14" r:id="rId3"/>
+    <hyperlink ref="N10" r:id="rId4"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId5"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: radio question added
</commit_message>
<xml_diff>
--- a/Quantium.Recruitment.Portal/wwwroot/QuestionsTemplate.xlsx
+++ b/Quantium.Recruitment.Portal/wwwroot/QuestionsTemplate.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="181" uniqueCount="128">
   <si>
     <t>Id</t>
   </si>
@@ -440,6 +440,9 @@
   </si>
   <si>
     <t>https://qjxnta.bl3302.livefilestore.com/y3mbPGVnlzCISN5I64XFRCEp_zwPHXkgdd_EIGt0xqSKXbq7rhQrrRGSUcyamcjenBxni79zrf9HCS6y4wYwBSSljHN8-DgTHbh2gh2f8dMdvrdZpy2iOpMqOpR8OkeZwWRZrBjamYNEDz_4UGEnGEjmt9EPrmR1PbbkoXmnNKv3vI?width=172&amp;height=144&amp;cropmode=none</t>
+  </si>
+  <si>
+    <t>IsRadio</t>
   </si>
 </sst>
 </file>
@@ -778,10 +781,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:O21"/>
+  <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="N12" sqref="N12"/>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="Q4" sqref="Q4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -797,7 +800,7 @@
     <col min="15" max="15" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -843,8 +846,11 @@
       <c r="O1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P1" s="1" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>1</v>
       </c>
@@ -878,8 +884,11 @@
       </c>
       <c r="N2" s="2"/>
       <c r="O2" s="1"/>
-    </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
+      <c r="P2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>2</v>
       </c>
@@ -916,7 +925,7 @@
       <c r="N3" s="2"/>
       <c r="O3" s="1"/>
     </row>
-    <row r="4" spans="1:15" ht="147" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:16" ht="147" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>3</v>
       </c>
@@ -957,7 +966,7 @@
       <c r="N4" s="2"/>
       <c r="O4" s="1"/>
     </row>
-    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>4</v>
       </c>
@@ -998,7 +1007,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1">
         <v>5</v>
       </c>
@@ -1043,7 +1052,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1">
         <v>6</v>
       </c>
@@ -1084,7 +1093,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>7</v>
       </c>
@@ -1125,7 +1134,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>8</v>
       </c>
@@ -1166,7 +1175,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="10" spans="1:15" ht="105" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:16" ht="105" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>9</v>
       </c>
@@ -1211,7 +1220,7 @@
       </c>
       <c r="O10" s="1"/>
     </row>
-    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>10</v>
       </c>
@@ -1250,7 +1259,7 @@
       <c r="N11" s="2"/>
       <c r="O11" s="1"/>
     </row>
-    <row r="12" spans="1:15" ht="150" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:16" ht="150" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>11</v>
       </c>
@@ -1289,7 +1298,7 @@
       <c r="N12" s="2"/>
       <c r="O12" s="1"/>
     </row>
-    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>12</v>
       </c>
@@ -1328,7 +1337,7 @@
       <c r="N13" s="2"/>
       <c r="O13" s="1"/>
     </row>
-    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>13</v>
       </c>
@@ -1369,7 +1378,7 @@
       </c>
       <c r="O14" s="1"/>
     </row>
-    <row r="15" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>14</v>
       </c>
@@ -1410,7 +1419,7 @@
       </c>
       <c r="O15" s="1"/>
     </row>
-    <row r="16" spans="1:15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>15</v>
       </c>

</xml_diff>

<commit_message>
fix: added new questions template with image column
</commit_message>
<xml_diff>
--- a/Quantium.Recruitment.Portal/wwwroot/QuestionsTemplate.xlsx
+++ b/Quantium.Recruitment.Portal/wwwroot/QuestionsTemplate.xlsx
@@ -2,14 +2,14 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+  <workbookPr autoCompressPictures="0" defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\QRecruitment\newcode\Quantium.Recruitment.Portal\wwwroot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Projects\QRecruitment-Phase1\Quantium.Recruitment.Portal\wwwroot\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11385"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11385" tabRatio="446"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,9 +65,6 @@
     <t>RandomizeOptions</t>
   </si>
   <si>
-    <t>ImageUrl</t>
-  </si>
-  <si>
     <t>QuestionGroup</t>
   </si>
   <si>
@@ -87,9 +84,6 @@
   </si>
   <si>
     <t>Hard</t>
-  </si>
-  <si>
-    <t>Can you implement multiple interfaces?</t>
   </si>
   <si>
     <t>YES</t>
@@ -444,11 +438,17 @@
   <si>
     <t>IsRadio</t>
   </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>Can you implement multiple interfaces?</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -516,6 +516,55 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="13858876" y="190500"/>
+          <a:ext cx="1352550" cy="800100"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -783,8 +832,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P21"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -796,7 +845,7 @@
     <col min="6" max="6" width="16.5703125" customWidth="1"/>
     <col min="8" max="8" width="11.28515625" customWidth="1"/>
     <col min="13" max="13" width="18.28515625" customWidth="1"/>
-    <col min="14" max="14" width="14" customWidth="1"/>
+    <col min="14" max="14" width="20.28515625" customWidth="1"/>
     <col min="15" max="15" width="20.5703125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -841,21 +890,21 @@
         <v>12</v>
       </c>
       <c r="N1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" s="1" t="s">
-        <v>14</v>
-      </c>
       <c r="P1" s="1" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>127</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" s="1">
-        <v>1</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>21</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>4</v>
@@ -864,20 +913,20 @@
         <v>20</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="G2" s="1"/>
       <c r="H2" s="1"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L2" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M2" s="1" t="b">
         <v>1</v>
@@ -893,7 +942,7 @@
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
@@ -902,22 +951,22 @@
         <v>172</v>
       </c>
       <c r="E3" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="G3" s="2" t="s">
         <v>25</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G3" s="2" t="s">
-        <v>27</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
       <c r="J3" s="1"/>
       <c r="K3" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L3" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M3" s="1" t="b">
         <v>1</v>
@@ -930,7 +979,7 @@
         <v>3</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -939,26 +988,26 @@
         <v>23</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="H4" s="1" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="J4" s="1"/>
       <c r="K4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L4" s="1" t="s">
         <v>19</v>
-      </c>
-      <c r="L4" s="1" t="s">
-        <v>20</v>
       </c>
       <c r="M4" s="1" t="b">
         <v>0</v>
@@ -971,40 +1020,40 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D5" s="1">
         <v>56</v>
       </c>
       <c r="E5" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="F5" s="1" t="s">
+      <c r="H5" s="2" t="s">
         <v>30</v>
-      </c>
-      <c r="G5" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>32</v>
       </c>
       <c r="I5" s="1"/>
       <c r="J5" s="1"/>
       <c r="K5" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L5" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M5" s="1" t="b">
         <v>1</v>
       </c>
       <c r="N5" s="2"/>
       <c r="O5" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
@@ -1012,44 +1061,44 @@
         <v>5</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D6" s="1">
         <v>172</v>
       </c>
       <c r="E6" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="F6" s="1" t="s">
+      <c r="H6" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="G6" s="1" t="s">
+      <c r="I6" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="H6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="I6" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>38</v>
-      </c>
       <c r="K6" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L6" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M6" s="1" t="b">
         <v>1</v>
       </c>
       <c r="N6" s="2"/>
       <c r="O6" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
@@ -1057,7 +1106,7 @@
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>4</v>
@@ -1066,31 +1115,31 @@
         <v>23</v>
       </c>
       <c r="E7" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="F7" s="1" t="s">
+      <c r="H7" s="2" t="s">
         <v>41</v>
-      </c>
-      <c r="G7" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="H7" s="2" t="s">
-        <v>43</v>
       </c>
       <c r="I7" s="1"/>
       <c r="J7" s="1"/>
       <c r="K7" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L7" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="M7" s="1" t="b">
         <v>1</v>
       </c>
       <c r="N7" s="2"/>
       <c r="O7" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
@@ -1098,40 +1147,40 @@
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="D8" s="1">
         <v>56</v>
       </c>
       <c r="E8" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="H8" s="2" t="s">
         <v>45</v>
-      </c>
-      <c r="G8" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>47</v>
       </c>
       <c r="I8" s="1"/>
       <c r="J8" s="1"/>
       <c r="K8" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L8" s="1" t="s">
         <v>16</v>
-      </c>
-      <c r="L8" s="1" t="s">
-        <v>17</v>
       </c>
       <c r="M8" s="1" t="b">
         <v>1</v>
       </c>
       <c r="N8" s="2"/>
       <c r="O8" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
@@ -1139,7 +1188,7 @@
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>4</v>
@@ -1148,31 +1197,31 @@
         <v>172</v>
       </c>
       <c r="E9" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="G9" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="F9" s="1" t="s">
+      <c r="H9" s="2" t="s">
         <v>50</v>
-      </c>
-      <c r="G9" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="H9" s="2" t="s">
-        <v>52</v>
       </c>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
       <c r="K9" s="1" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M9" s="1" t="b">
         <v>1</v>
       </c>
       <c r="N9" s="2"/>
       <c r="O9" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:16" ht="105" x14ac:dyDescent="0.25">
@@ -1180,7 +1229,7 @@
         <v>9</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>5</v>
@@ -1189,10 +1238,10 @@
         <v>23</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G10" s="1">
         <v>4</v>
@@ -1207,16 +1256,16 @@
         <v>10</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M10" s="1" t="b">
         <v>1</v>
       </c>
       <c r="N10" s="5" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="O10" s="1"/>
     </row>
@@ -1225,7 +1274,7 @@
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>6</v>
@@ -1234,24 +1283,24 @@
         <v>56</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="F11" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="H11" s="2" t="s">
         <v>62</v>
-      </c>
-      <c r="F11" s="3" t="s">
-        <v>63</v>
-      </c>
-      <c r="G11" s="1" t="s">
-        <v>65</v>
-      </c>
-      <c r="H11" s="2" t="s">
-        <v>64</v>
       </c>
       <c r="I11" s="1"/>
       <c r="J11" s="1"/>
       <c r="K11" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L11" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M11" s="1" t="b">
         <v>1</v>
@@ -1264,7 +1313,7 @@
         <v>11</v>
       </c>
       <c r="B12" s="3" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>7</v>
@@ -1273,24 +1322,24 @@
         <v>172</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="G12" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="H12" s="1" t="s">
         <v>68</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>70</v>
       </c>
       <c r="I12" s="1"/>
       <c r="J12" s="1"/>
       <c r="K12" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="L12" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M12" s="1" t="b">
         <v>1</v>
@@ -1303,7 +1352,7 @@
         <v>12</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>7</v>
@@ -1312,24 +1361,24 @@
         <v>23</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="G13" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="H13" s="2" t="s">
         <v>73</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="H13" s="2" t="s">
-        <v>75</v>
       </c>
       <c r="I13" s="1"/>
       <c r="J13" s="1"/>
       <c r="K13" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="L13" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M13" s="1" t="b">
         <v>1</v>
@@ -1342,7 +1391,7 @@
         <v>13</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>6</v>
@@ -1357,24 +1406,24 @@
         <v>0</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="I14" s="1"/>
       <c r="J14" s="1"/>
       <c r="K14" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="L14" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M14" s="1" t="b">
         <v>1</v>
       </c>
       <c r="N14" s="5" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="O14" s="1"/>
     </row>
@@ -1383,7 +1432,7 @@
         <v>14</v>
       </c>
       <c r="B15" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>7</v>
@@ -1392,30 +1441,30 @@
         <v>172</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="F15" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="G15" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="H15" s="2" t="s">
         <v>82</v>
-      </c>
-      <c r="G15" s="1" t="s">
-        <v>83</v>
-      </c>
-      <c r="H15" s="2" t="s">
-        <v>84</v>
       </c>
       <c r="I15" s="1"/>
       <c r="J15" s="1"/>
       <c r="K15" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="L15" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M15" s="1" t="b">
         <v>1</v>
       </c>
       <c r="N15" s="5" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="O15" s="1"/>
     </row>
@@ -1424,7 +1473,7 @@
         <v>15</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>4</v>
@@ -1433,34 +1482,34 @@
         <v>23</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="G16" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="H16" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="I16" s="1" t="s">
         <v>89</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>91</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>92</v>
-      </c>
       <c r="K16" s="1" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="L16" s="1" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="M16" s="1" t="b">
         <v>1</v>
       </c>
       <c r="N16" s="5" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="O16" s="1"/>
     </row>
@@ -1469,7 +1518,7 @@
         <v>16</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>7</v>
@@ -1478,24 +1527,24 @@
         <v>56</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="G17" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="H17" s="2" t="s">
         <v>95</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>96</v>
-      </c>
-      <c r="H17" s="2" t="s">
-        <v>97</v>
       </c>
       <c r="I17" s="1"/>
       <c r="J17" s="1"/>
       <c r="K17" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L17" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M17" s="1" t="b">
         <v>1</v>
@@ -1508,37 +1557,37 @@
         <v>17</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D18" s="1">
         <v>172</v>
       </c>
       <c r="E18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="F18" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="G18" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="H18" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="I18" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>60</v>
-      </c>
-      <c r="H18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="I18" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="J18" s="1" t="s">
-        <v>102</v>
-      </c>
       <c r="K18" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L18" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M18" s="1" t="b">
         <v>1</v>
@@ -1551,7 +1600,7 @@
         <v>18</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>4</v>
@@ -1569,15 +1618,15 @@
         <v>4</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="I19" s="1"/>
       <c r="J19" s="1"/>
       <c r="K19" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L19" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M19" s="1" t="b">
         <v>0</v>
@@ -1590,7 +1639,7 @@
         <v>19</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>6</v>
@@ -1599,24 +1648,24 @@
         <v>56</v>
       </c>
       <c r="E20" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="F20" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="G20" s="1" t="s">
         <v>109</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="H20" s="3" t="s">
         <v>110</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>111</v>
-      </c>
-      <c r="H20" s="3" t="s">
-        <v>112</v>
       </c>
       <c r="I20" s="1"/>
       <c r="J20" s="1"/>
       <c r="K20" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L20" s="1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="M20" s="1" t="b">
         <v>1</v>
@@ -1629,7 +1678,7 @@
         <v>20</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="C21" s="1" t="s">
         <v>6</v>
@@ -1638,24 +1687,24 @@
         <v>172</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="F21" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G21" s="1">
         <v>2</v>
       </c>
       <c r="H21" s="3" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="I21" s="1"/>
       <c r="J21" s="1"/>
       <c r="K21" s="1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="L21" s="1" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="M21" s="1" t="b">
         <v>0</v>
@@ -1665,12 +1714,13 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="N16" r:id="rId1"/>
-    <hyperlink ref="N15" r:id="rId2"/>
-    <hyperlink ref="N14" r:id="rId3"/>
-    <hyperlink ref="N10" r:id="rId4"/>
+    <hyperlink ref="N10" r:id="rId1"/>
+    <hyperlink ref="N14" r:id="rId2"/>
+    <hyperlink ref="N15" r:id="rId3"/>
+    <hyperlink ref="N16" r:id="rId4"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId5"/>
+  <drawing r:id="rId6"/>
 </worksheet>
 </file>
</xml_diff>